<commit_message>
IN CASE I DO ANYTHING ON WEEKEND TIME FOR LEARN
</commit_message>
<xml_diff>
--- a/bom/BOM_Sample.xlsx
+++ b/bom/BOM_Sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DC202" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="402">
   <si>
     <t>DC202</t>
   </si>
@@ -1162,6 +1162,90 @@
   </si>
   <si>
     <t>DC202 Drawn in Fusion360 AND Inventor</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Turck</t>
+  </si>
+  <si>
+    <t>Not sure</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>110AS002</t>
+  </si>
+  <si>
+    <t>110AS003</t>
+  </si>
+  <si>
+    <t>110AS004</t>
+  </si>
+  <si>
+    <t>110AS005</t>
+  </si>
+  <si>
+    <t>110AS006</t>
+  </si>
+  <si>
+    <t>110AS007</t>
+  </si>
+  <si>
+    <t>110AS008</t>
+  </si>
+  <si>
+    <t>110AS009</t>
+  </si>
+  <si>
+    <t>110AS010</t>
+  </si>
+  <si>
+    <t>110AS011</t>
+  </si>
+  <si>
+    <t>110AS012</t>
+  </si>
+  <si>
+    <t>110AS013</t>
+  </si>
+  <si>
+    <t>110AS014</t>
+  </si>
+  <si>
+    <t>Spacer</t>
+  </si>
+  <si>
+    <t>Fiberglass gimbal rail</t>
+  </si>
+  <si>
+    <t>mtg plate</t>
+  </si>
+  <si>
+    <t>tower piece</t>
+  </si>
+  <si>
+    <t>roll</t>
+  </si>
+  <si>
+    <t>axle</t>
+  </si>
+  <si>
+    <t>adaopter</t>
+  </si>
+  <si>
+    <t>cnc part</t>
+  </si>
+  <si>
+    <t>3d print</t>
+  </si>
+  <si>
+    <t>purchased pulley</t>
+  </si>
+  <si>
+    <t>purchased part</t>
   </si>
 </sst>
 </file>
@@ -2183,8 +2267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,7 +2409,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,7 +2420,6 @@
     <col min="4" max="4" width="11.140625" style="91" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2364,14 +2447,14 @@
       <c r="D2" s="94" t="s">
         <v>259</v>
       </c>
-      <c r="E2" s="110" t="s">
+      <c r="E2" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="110" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="95" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2387,14 +2470,14 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4">
-        <v>1</v>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>15</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
       </c>
       <c r="H3" s="116" t="s">
         <v>263</v>
@@ -2413,11 +2496,13 @@
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
       <c r="H4" s="116" t="s">
         <v>263</v>
       </c>
@@ -2435,14 +2520,14 @@
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4">
-        <v>1</v>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>15</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
       </c>
       <c r="H5" s="116" t="s">
         <v>263</v>
@@ -2461,11 +2546,13 @@
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
       <c r="H6" s="116" t="s">
         <v>263</v>
       </c>
@@ -2481,9 +2568,11 @@
         <v>262</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G7" s="4"/>
       <c r="H7" s="116" t="s">
         <v>263</v>
       </c>
@@ -2499,9 +2588,9 @@
         <v>262</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="116" t="s">
         <v>263</v>
       </c>
@@ -2545,7 +2634,6 @@
       <c r="F13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="91"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -2566,7 +2654,6 @@
       <c r="F14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="91"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -2587,7 +2674,6 @@
       <c r="F15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="91"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -2608,9 +2694,8 @@
       <c r="F16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="91"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>11</v>
       </c>
@@ -2629,9 +2714,8 @@
       <c r="F17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="91"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>12</v>
       </c>
@@ -2650,9 +2734,8 @@
       <c r="F18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="91"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>13</v>
       </c>
@@ -2671,9 +2754,8 @@
       <c r="F19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="91"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>14</v>
       </c>
@@ -2692,9 +2774,8 @@
       <c r="F20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="91"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>15</v>
       </c>
@@ -2713,9 +2794,8 @@
       <c r="F21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="91"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>16</v>
       </c>
@@ -2734,9 +2814,8 @@
       <c r="F22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="91"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>17</v>
       </c>
@@ -2755,9 +2834,8 @@
       <c r="F23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="91"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>18</v>
       </c>
@@ -2773,10 +2851,11 @@
       <c r="E24" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="91"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>19</v>
       </c>
@@ -2792,27 +2871,31 @@
       <c r="E25" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="91"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>20</v>
       </c>
       <c r="B26" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="28"/>
+      <c r="C26" s="28" t="s">
+        <v>376</v>
+      </c>
       <c r="D26" s="4">
         <v>1</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="F26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="91"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>21</v>
       </c>
@@ -2831,9 +2914,8 @@
       <c r="F27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="91"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>22</v>
       </c>
@@ -2852,9 +2934,8 @@
       <c r="F28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="91"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>23</v>
       </c>
@@ -2873,26 +2954,28 @@
       <c r="F29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G29" s="91"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>24</v>
       </c>
       <c r="B30" s="98" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="28"/>
+      <c r="C30" s="28" t="s">
+        <v>376</v>
+      </c>
       <c r="D30" s="4">
         <v>2</v>
       </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="F30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="91"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>25</v>
       </c>
@@ -2911,7 +2994,6 @@
       <c r="F31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="91"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2934,8 +3016,8 @@
   </sheetPr>
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2973,14 +3055,14 @@
       <c r="D2" s="94" t="s">
         <v>259</v>
       </c>
-      <c r="E2" s="110" t="s">
+      <c r="E2" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="110" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="95" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2990,15 +3072,19 @@
       <c r="B3" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>391</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E3" s="4">
-        <v>1</v>
+      <c r="E3" s="1" t="s">
+        <v>378</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
       <c r="H3" s="90" t="s">
         <v>263</v>
       </c>
@@ -3010,15 +3096,19 @@
       <c r="B4" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>392</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="4">
         <v>2</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
       <c r="H4" s="90" t="s">
         <v>263</v>
       </c>
@@ -3030,15 +3120,19 @@
       <c r="B5" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>393</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="4">
         <v>2</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
       <c r="H5" s="90" t="s">
         <v>263</v>
       </c>
@@ -3050,15 +3144,19 @@
       <c r="B6" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>394</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="4">
         <v>4</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
       <c r="H6" s="90" t="s">
         <v>263</v>
       </c>
@@ -3070,15 +3168,19 @@
       <c r="B7" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>395</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="4">
-        <v>1</v>
+      <c r="E7" s="1" t="s">
+        <v>382</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
       <c r="H7" s="90" t="s">
         <v>263</v>
       </c>
@@ -3090,15 +3192,19 @@
       <c r="B8" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>396</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="4">
-        <v>1</v>
+      <c r="E8" s="1" t="s">
+        <v>383</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
       <c r="H8" s="90" t="s">
         <v>263</v>
       </c>
@@ -3110,15 +3216,19 @@
       <c r="B9" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="4">
-        <v>1</v>
+      <c r="E9" s="1" t="s">
+        <v>384</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
       <c r="H9" s="90" t="s">
         <v>263</v>
       </c>
@@ -3130,15 +3240,19 @@
       <c r="B10" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>400</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="4">
-        <v>1</v>
+      <c r="E10" s="1" t="s">
+        <v>385</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
       <c r="H10" s="90" t="s">
         <v>263</v>
       </c>
@@ -3150,15 +3264,19 @@
       <c r="B11" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>401</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="4">
-        <v>1</v>
+      <c r="E11" s="1" t="s">
+        <v>386</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
       <c r="H11" s="90" t="s">
         <v>263</v>
       </c>
@@ -3170,15 +3288,19 @@
       <c r="B12" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>398</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E12" s="4">
-        <v>1</v>
+      <c r="E12" s="1" t="s">
+        <v>387</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
       <c r="H12" s="90" t="s">
         <v>263</v>
       </c>
@@ -3190,15 +3312,19 @@
       <c r="B13" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>398</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="4">
-        <v>1</v>
+      <c r="E13" s="1" t="s">
+        <v>388</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
       <c r="H13" s="90" t="s">
         <v>263</v>
       </c>
@@ -3210,15 +3336,19 @@
       <c r="B14" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>398</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E14" s="4">
-        <v>1</v>
+      <c r="E14" s="1" t="s">
+        <v>389</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
       <c r="H14" s="90" t="s">
         <v>263</v>
       </c>
@@ -3230,15 +3360,19 @@
       <c r="B15" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>399</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="4">
         <v>2</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
       <c r="H15" s="90" t="s">
         <v>263</v>
       </c>
@@ -3250,15 +3384,17 @@
       <c r="B16" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>398</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="4">
-        <v>1</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
       <c r="H16" s="90" t="s">
         <v>263</v>
       </c>

</xml_diff>